<commit_message>
add custom cl argument type, do refactoring
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="104">
   <si>
     <t>Температура min..max</t>
   </si>
@@ -34,253 +34,298 @@
     <t>Направление</t>
   </si>
   <si>
-    <t>18 сентября вт</t>
+    <t>19 сентября ср</t>
+  </si>
+  <si>
+    <t>ночь+17+18</t>
+  </si>
+  <si>
+    <t>ясно</t>
+  </si>
+  <si>
+    <t>752…754</t>
+  </si>
+  <si>
+    <t>76…81</t>
+  </si>
+  <si>
+    <t>3…5</t>
+  </si>
+  <si>
+    <t>ю-з</t>
+  </si>
+  <si>
+    <t>утро+18+19</t>
+  </si>
+  <si>
+    <t>73…78</t>
+  </si>
+  <si>
+    <t>4…6</t>
+  </si>
+  <si>
+    <t>день+25+26</t>
+  </si>
+  <si>
+    <t>751…753</t>
+  </si>
+  <si>
+    <t>50…55</t>
+  </si>
+  <si>
+    <t>вечер+19+20</t>
+  </si>
+  <si>
+    <t>74…79</t>
+  </si>
+  <si>
+    <t>2…4</t>
+  </si>
+  <si>
+    <t>20 сентября чт</t>
+  </si>
+  <si>
+    <t>ночь+15+16</t>
+  </si>
+  <si>
+    <t>91…96</t>
+  </si>
+  <si>
+    <t>0…2</t>
+  </si>
+  <si>
+    <t>с-з</t>
+  </si>
+  <si>
+    <t>утро+17+18</t>
+  </si>
+  <si>
+    <t>85…90</t>
+  </si>
+  <si>
+    <t>ю</t>
+  </si>
+  <si>
+    <t>день+26+27</t>
+  </si>
+  <si>
+    <t>48…53</t>
+  </si>
+  <si>
+    <t>вечер+20+21</t>
+  </si>
+  <si>
+    <t>1…3</t>
+  </si>
+  <si>
+    <t>21 сентября пт</t>
+  </si>
+  <si>
+    <t>78…83</t>
+  </si>
+  <si>
+    <t>749…751</t>
+  </si>
+  <si>
+    <t>43…48</t>
+  </si>
+  <si>
+    <t>747…749</t>
+  </si>
+  <si>
+    <t>54…59</t>
+  </si>
+  <si>
+    <t>22 сентября сб</t>
+  </si>
+  <si>
+    <t>ночь+18+19</t>
+  </si>
+  <si>
+    <t>745…747</t>
+  </si>
+  <si>
+    <t>60…65</t>
+  </si>
+  <si>
+    <t>5…7</t>
+  </si>
+  <si>
+    <t>утро+15+16</t>
+  </si>
+  <si>
+    <t>пасмурно, кратковременный дождь</t>
+  </si>
+  <si>
+    <t>746…748</t>
+  </si>
+  <si>
+    <t>день+14+15</t>
+  </si>
+  <si>
+    <t>з</t>
+  </si>
+  <si>
+    <t>вечер+12+13</t>
+  </si>
+  <si>
+    <t>малооблачно</t>
+  </si>
+  <si>
+    <t>23 сентября вс</t>
+  </si>
+  <si>
+    <t>ночь+10+11</t>
+  </si>
+  <si>
+    <t>68…73</t>
+  </si>
+  <si>
+    <t>утро+10+11</t>
+  </si>
+  <si>
+    <t>75…80</t>
+  </si>
+  <si>
+    <t>день+15+16</t>
+  </si>
+  <si>
+    <t>облачно</t>
+  </si>
+  <si>
+    <t>750…752</t>
+  </si>
+  <si>
+    <t>44…49</t>
+  </si>
+  <si>
+    <t>6…8</t>
+  </si>
+  <si>
+    <t>58…63</t>
+  </si>
+  <si>
+    <t>24 сентября пн</t>
+  </si>
+  <si>
+    <t>ночь+8+9</t>
+  </si>
+  <si>
+    <t>748…750</t>
+  </si>
+  <si>
+    <t>71…76</t>
+  </si>
+  <si>
+    <t>утро+9+10</t>
+  </si>
+  <si>
+    <t>744…746</t>
+  </si>
+  <si>
+    <t>64…69</t>
+  </si>
+  <si>
+    <t>день+10+11</t>
+  </si>
+  <si>
+    <t>738…740</t>
+  </si>
+  <si>
+    <t>79…84</t>
+  </si>
+  <si>
+    <t>облачно, кратковременный дождь</t>
+  </si>
+  <si>
+    <t>736…738</t>
+  </si>
+  <si>
+    <t>87…92</t>
+  </si>
+  <si>
+    <t>25 сентября вт</t>
   </si>
   <si>
     <t>ночь+12+13</t>
   </si>
   <si>
-    <t>ясно</t>
-  </si>
-  <si>
-    <t>752…754</t>
-  </si>
-  <si>
-    <t>72…77</t>
-  </si>
-  <si>
-    <t>3…5</t>
-  </si>
-  <si>
-    <t>ю-з</t>
-  </si>
-  <si>
-    <t>утро+15+16</t>
-  </si>
-  <si>
-    <t>68…73</t>
-  </si>
-  <si>
-    <t>з</t>
-  </si>
-  <si>
-    <t>день+20+21</t>
-  </si>
-  <si>
-    <t>малооблачно</t>
-  </si>
-  <si>
-    <t>751…753</t>
+    <t>735…737</t>
+  </si>
+  <si>
+    <t>90…95</t>
+  </si>
+  <si>
+    <t>утро+12+13</t>
+  </si>
+  <si>
+    <t>734…736</t>
+  </si>
+  <si>
+    <t>737…739</t>
   </si>
   <si>
     <t>57…62</t>
   </si>
   <si>
-    <t>4…6</t>
-  </si>
-  <si>
-    <t>вечер+15+16</t>
-  </si>
-  <si>
-    <t>79…84</t>
-  </si>
-  <si>
-    <t>2…4</t>
-  </si>
-  <si>
-    <t>19 сентября ср</t>
-  </si>
-  <si>
-    <t>87…92</t>
-  </si>
-  <si>
-    <t>1…3</t>
-  </si>
-  <si>
-    <t>утро+16+17</t>
-  </si>
-  <si>
-    <t>76…81</t>
-  </si>
-  <si>
-    <t>день+24+25</t>
-  </si>
-  <si>
-    <t>51…56</t>
-  </si>
-  <si>
-    <t>вечер+18+19</t>
-  </si>
-  <si>
-    <t>750…752</t>
-  </si>
-  <si>
-    <t>20 сентября чт</t>
-  </si>
-  <si>
-    <t>ночь+15+16</t>
-  </si>
-  <si>
-    <t>78…83</t>
-  </si>
-  <si>
-    <t>утро+18+19</t>
-  </si>
-  <si>
-    <t>день+25+26</t>
-  </si>
-  <si>
-    <t>56…61</t>
-  </si>
-  <si>
-    <t>21 сентября пт</t>
-  </si>
-  <si>
-    <t>93…98</t>
-  </si>
-  <si>
-    <t>0…2</t>
-  </si>
-  <si>
-    <t>ю</t>
-  </si>
-  <si>
-    <t>50…55</t>
-  </si>
-  <si>
-    <t>вечер+17+18</t>
-  </si>
-  <si>
-    <t>22 сентября сб</t>
-  </si>
-  <si>
-    <t>ночь+17+18</t>
-  </si>
-  <si>
-    <t>749…751</t>
-  </si>
-  <si>
-    <t>73…78</t>
-  </si>
-  <si>
-    <t>748…750</t>
-  </si>
-  <si>
-    <t>70…75</t>
-  </si>
-  <si>
-    <t>746…748</t>
-  </si>
-  <si>
-    <t>43…48</t>
-  </si>
-  <si>
-    <t>5…7</t>
-  </si>
-  <si>
-    <t>747…749</t>
-  </si>
-  <si>
-    <t>81…86</t>
-  </si>
-  <si>
-    <t>с-з</t>
-  </si>
-  <si>
-    <t>23 сентября вс</t>
-  </si>
-  <si>
-    <t>ночь+13+14</t>
-  </si>
-  <si>
-    <t>пасмурно, кратковременный дождь</t>
-  </si>
-  <si>
-    <t>утро+9+10</t>
-  </si>
-  <si>
-    <t>85…90</t>
+    <t>7…9</t>
+  </si>
+  <si>
+    <t>вечер+10+11</t>
+  </si>
+  <si>
+    <t>739…741</t>
+  </si>
+  <si>
+    <t>82…87</t>
+  </si>
+  <si>
+    <t>26 сентября ср</t>
+  </si>
+  <si>
+    <t>ночь+9+10</t>
+  </si>
+  <si>
+    <t>740…742</t>
+  </si>
+  <si>
+    <t>день+13+14</t>
+  </si>
+  <si>
+    <t>742…744</t>
+  </si>
+  <si>
+    <t>с</t>
+  </si>
+  <si>
+    <t>вечер+11+12</t>
+  </si>
+  <si>
+    <t>27 сентября чт</t>
+  </si>
+  <si>
+    <t>пасмурно</t>
+  </si>
+  <si>
+    <t>84…89</t>
   </si>
   <si>
     <t>день+12+13</t>
   </si>
   <si>
-    <t>745…747</t>
-  </si>
-  <si>
-    <t>84…89</t>
-  </si>
-  <si>
-    <t>вечер+10+11</t>
-  </si>
-  <si>
-    <t>малооблачно, кратковременный дождь</t>
-  </si>
-  <si>
-    <t>24 сентября пн</t>
-  </si>
-  <si>
-    <t>ночь+8+9</t>
-  </si>
-  <si>
-    <t>74…79</t>
-  </si>
-  <si>
-    <t>день+13+14</t>
-  </si>
-  <si>
-    <t>пасмурно</t>
-  </si>
-  <si>
-    <t>743…745</t>
-  </si>
-  <si>
-    <t>47…52</t>
-  </si>
-  <si>
-    <t>вечер+9+10</t>
-  </si>
-  <si>
-    <t>740…742</t>
-  </si>
-  <si>
-    <t>25 сентября вт</t>
-  </si>
-  <si>
-    <t>ночь+9+10</t>
-  </si>
-  <si>
-    <t>с</t>
-  </si>
-  <si>
-    <t>облачно</t>
-  </si>
-  <si>
-    <t>53…58</t>
-  </si>
-  <si>
-    <t>26 сентября ср</t>
-  </si>
-  <si>
-    <t>утро+10+11</t>
+    <t>753…755</t>
   </si>
   <si>
     <t>65…70</t>
   </si>
   <si>
-    <t>день+16+17</t>
-  </si>
-  <si>
-    <t>744…746</t>
-  </si>
-  <si>
-    <t>52…57</t>
-  </si>
-  <si>
-    <t>6…8</t>
-  </si>
-  <si>
-    <t>вечер+13+14</t>
+    <t>вечер+8+9</t>
+  </si>
+  <si>
+    <t>756…758</t>
+  </si>
+  <si>
+    <t>83…88</t>
   </si>
 </sst>
 </file>
@@ -627,7 +672,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="15.7109375" customWidth="1"/>
+    <col min="1" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -689,10 +734,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -700,49 +745,49 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -751,13 +796,13 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -774,47 +819,47 @@
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -822,597 +867,597 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
         <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
         <v>79</v>
       </c>
-      <c r="C48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" t="s">
-        <v>50</v>
-      </c>
       <c r="E48" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E51" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E53" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="E54" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F54" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>